<commit_message>
Analysis Specification edit screen is less confusing
close #67
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test.xlsx
+++ b/bika/lims/setupdata/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="752" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="13" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="969" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4676" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4526" uniqueCount="1131">
   <si>
     <t>Password lifetime</t>
   </si>
@@ -3574,7 +3574,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -3598,10 +3598,6 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="44">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
@@ -3623,7 +3619,7 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="165" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -3736,14 +3732,13 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
     <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
     <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="15"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3816,11 +3811,11 @@
   <dimension ref="A2:N4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B4" activeCellId="1" pane="topLeft" sqref="A17:G66 B4"/>
+      <selection activeCell="B4" activeCellId="0" pane="topLeft" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2" s="2"/>
@@ -3928,15 +3923,15 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="20.0980392156863"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="39.3607843137255"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="18.756862745098"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="8" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="20.1960784313725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="39.5607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="18.8470588235294"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="8" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="9">
@@ -4757,13 +4752,13 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="31" width="33.1647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="31" width="51.4156862745098"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="31" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="31" width="33.3294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="31" width="51.6705882352941"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="31" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="32">
@@ -4910,14 +4905,14 @@
   <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B1" activeCellId="1" pane="topLeft" sqref="A17:G66 B1"/>
+      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="81.7333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="23.6156862745098"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="8" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="82.1411764705882"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="23.7333333333333"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="8" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="9">
@@ -5143,19 +5138,19 @@
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="G1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="bottomLeft" topLeftCell="A248" xSplit="0" ySplit="1185"/>
       <selection activeCell="G1" activeCellId="0" pane="topLeft" sqref="G1"/>
-      <selection activeCell="Q263" activeCellId="1" pane="bottomLeft" sqref="A17:G66 Q263"/>
+      <selection activeCell="Q263" activeCellId="0" pane="bottomLeft" sqref="Q263"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="21" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="34" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="20" min="8" style="21" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="34" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="21" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="18" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="21" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="28" min="25" style="8" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="257" min="29" style="28" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="21" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="34" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="20" min="8" style="21" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="34" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="21" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="18" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="21" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="28" min="25" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="257" min="29" style="28" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24.25" outlineLevel="0" r="1" s="23">
@@ -7052,7 +7047,7 @@
         <v>781</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="74">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="74">
       <c r="A74" s="21" t="s">
         <v>816</v>
       </c>
@@ -11858,16 +11853,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2159"/>
+  <dimension ref="A1:E2012"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A2129" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2164" activeCellId="1" pane="topLeft" sqref="A17:G66 A2164"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1963" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E2009" activeCellId="0" pane="topLeft" sqref="E2009"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="21" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="227" min="4" style="28" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="257" min="228" style="0" width="10.7254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="21" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="227" min="4" style="28" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="257" min="228" style="0" width="10.7803921568627"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24.25" outlineLevel="0" r="1" s="23">
@@ -33440,7 +33435,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1474">
       <c r="A1474" s="18" t="s">
-        <v>653</v>
+        <v>572</v>
       </c>
       <c r="B1474" s="21" t="s">
         <v>839</v>
@@ -33498,7 +33493,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1478">
-      <c r="A1478" s="18"/>
       <c r="B1478" s="21" t="s">
         <v>795</v>
       </c>
@@ -34142,7 +34136,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1523">
       <c r="A1523" s="18" t="s">
-        <v>572</v>
+        <v>659</v>
       </c>
       <c r="B1523" s="21" t="s">
         <v>839</v>
@@ -34214,7 +34208,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1528">
-      <c r="A1528" s="18"/>
       <c r="B1528" s="21" t="s">
         <v>865</v>
       </c>
@@ -34229,7 +34222,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1529">
-      <c r="A1529" s="18"/>
       <c r="B1529" s="21" t="s">
         <v>815</v>
       </c>
@@ -34843,7 +34835,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1572">
       <c r="A1572" s="18" t="s">
-        <v>656</v>
+        <v>664</v>
       </c>
       <c r="B1572" s="21" t="s">
         <v>839</v>
@@ -34859,6 +34851,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1573">
+      <c r="A1573" s="18"/>
       <c r="B1573" s="21" t="s">
         <v>787</v>
       </c>
@@ -34873,6 +34866,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1574">
+      <c r="A1574" s="18"/>
       <c r="B1574" s="21" t="s">
         <v>876</v>
       </c>
@@ -34887,6 +34881,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1575">
+      <c r="A1575" s="18"/>
       <c r="B1575" s="21" t="s">
         <v>790</v>
       </c>
@@ -34901,6 +34896,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1576">
+      <c r="A1576" s="18"/>
       <c r="B1576" s="21" t="s">
         <v>795</v>
       </c>
@@ -34915,6 +34911,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1577">
+      <c r="A1577" s="18"/>
       <c r="B1577" s="21" t="s">
         <v>865</v>
       </c>
@@ -34989,7 +34986,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1582">
-      <c r="A1582" s="18"/>
       <c r="B1582" s="21" t="s">
         <v>802</v>
       </c>
@@ -35004,7 +35000,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1583">
-      <c r="A1583" s="18"/>
       <c r="B1583" s="21" t="s">
         <v>849</v>
       </c>
@@ -35019,7 +35014,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1584">
-      <c r="A1584" s="18"/>
       <c r="B1584" s="21" t="s">
         <v>863</v>
       </c>
@@ -35034,7 +35028,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1585">
-      <c r="A1585" s="18"/>
       <c r="B1585" s="21" t="s">
         <v>805</v>
       </c>
@@ -35049,7 +35042,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1586">
-      <c r="A1586" s="18"/>
       <c r="B1586" s="21" t="s">
         <v>890</v>
       </c>
@@ -35064,7 +35056,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1587">
-      <c r="A1587" s="18"/>
       <c r="B1587" s="21" t="s">
         <v>14</v>
       </c>
@@ -35079,7 +35070,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1588">
-      <c r="A1588" s="18"/>
       <c r="B1588" s="21" t="s">
         <v>910</v>
       </c>
@@ -35543,7 +35533,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1621">
       <c r="A1621" s="18" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="B1621" s="21" t="s">
         <v>839</v>
@@ -35587,6 +35577,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1624">
+      <c r="A1624" s="18"/>
       <c r="B1624" s="21" t="s">
         <v>790</v>
       </c>
@@ -35601,6 +35592,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1625">
+      <c r="A1625" s="18"/>
       <c r="B1625" s="21" t="s">
         <v>795</v>
       </c>
@@ -35615,6 +35607,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1626">
+      <c r="A1626" s="18"/>
       <c r="B1626" s="21" t="s">
         <v>865</v>
       </c>
@@ -35629,6 +35622,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1627">
+      <c r="A1627" s="18"/>
       <c r="B1627" s="21" t="s">
         <v>815</v>
       </c>
@@ -35688,7 +35682,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1631">
-      <c r="A1631" s="18"/>
       <c r="B1631" s="21" t="s">
         <v>802</v>
       </c>
@@ -35703,7 +35696,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1632">
-      <c r="A1632" s="18"/>
       <c r="B1632" s="21" t="s">
         <v>849</v>
       </c>
@@ -35718,7 +35710,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1633">
-      <c r="A1633" s="18"/>
       <c r="B1633" s="21" t="s">
         <v>863</v>
       </c>
@@ -35733,7 +35724,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1634">
-      <c r="A1634" s="18"/>
       <c r="B1634" s="21" t="s">
         <v>805</v>
       </c>
@@ -35748,7 +35738,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1635">
-      <c r="A1635" s="18"/>
       <c r="B1635" s="21" t="s">
         <v>890</v>
       </c>
@@ -35763,7 +35752,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1636">
-      <c r="A1636" s="18"/>
       <c r="B1636" s="21" t="s">
         <v>14</v>
       </c>
@@ -35778,7 +35766,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1637">
-      <c r="A1637" s="18"/>
       <c r="B1637" s="21" t="s">
         <v>910</v>
       </c>
@@ -36240,9 +36227,9 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1670">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="1670">
       <c r="A1670" s="18" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B1670" s="21" t="s">
         <v>839</v>
@@ -36258,7 +36245,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1671">
-      <c r="A1671" s="18"/>
       <c r="B1671" s="21" t="s">
         <v>787</v>
       </c>
@@ -36273,7 +36259,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1672">
-      <c r="A1672" s="18"/>
       <c r="B1672" s="21" t="s">
         <v>876</v>
       </c>
@@ -36288,7 +36273,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1673">
-      <c r="A1673" s="18"/>
       <c r="B1673" s="21" t="s">
         <v>790</v>
       </c>
@@ -36940,7 +36924,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1719">
       <c r="A1719" s="18" t="s">
-        <v>589</v>
+        <v>647</v>
       </c>
       <c r="B1719" s="21" t="s">
         <v>839</v>
@@ -36970,7 +36954,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1721">
-      <c r="A1721" s="18"/>
       <c r="B1721" s="21" t="s">
         <v>876</v>
       </c>
@@ -36985,7 +36968,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1722">
-      <c r="A1722" s="18"/>
       <c r="B1722" s="21" t="s">
         <v>790</v>
       </c>
@@ -37000,7 +36982,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1723">
-      <c r="A1723" s="18"/>
       <c r="B1723" s="21" t="s">
         <v>795</v>
       </c>
@@ -37637,7 +37618,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1768">
       <c r="A1768" s="18" t="s">
-        <v>662</v>
+        <v>592</v>
       </c>
       <c r="B1768" s="21" t="s">
         <v>839</v>
@@ -37681,7 +37662,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1771">
-      <c r="A1771" s="18"/>
       <c r="B1771" s="21" t="s">
         <v>790</v>
       </c>
@@ -37696,7 +37676,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1772">
-      <c r="A1772" s="18"/>
       <c r="B1772" s="21" t="s">
         <v>795</v>
       </c>
@@ -37711,7 +37690,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1773">
-      <c r="A1773" s="18"/>
       <c r="B1773" s="21" t="s">
         <v>865</v>
       </c>
@@ -38331,9 +38309,9 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="1817">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1817">
       <c r="A1817" s="18" t="s">
-        <v>666</v>
+        <v>595</v>
       </c>
       <c r="B1817" s="21" t="s">
         <v>839</v>
@@ -38391,7 +38369,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1821">
-      <c r="A1821" s="18"/>
       <c r="B1821" s="21" t="s">
         <v>795</v>
       </c>
@@ -38406,7 +38383,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1822">
-      <c r="A1822" s="18"/>
       <c r="B1822" s="21" t="s">
         <v>865</v>
       </c>
@@ -38421,7 +38397,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1823">
-      <c r="A1823" s="18"/>
       <c r="B1823" s="21" t="s">
         <v>815</v>
       </c>
@@ -39028,7 +39003,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1866">
       <c r="A1866" s="18" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="B1866" s="21" t="s">
         <v>839</v>
@@ -39100,7 +39075,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1871">
-      <c r="A1871" s="18"/>
       <c r="B1871" s="21" t="s">
         <v>865</v>
       </c>
@@ -39115,7 +39089,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1872">
-      <c r="A1872" s="18"/>
       <c r="B1872" s="21" t="s">
         <v>815</v>
       </c>
@@ -39130,7 +39103,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1873">
-      <c r="A1873" s="18"/>
       <c r="B1873" s="21" t="s">
         <v>799</v>
       </c>
@@ -39722,7 +39694,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1915">
       <c r="A1915" s="18" t="s">
-        <v>592</v>
+        <v>669</v>
       </c>
       <c r="B1915" s="21" t="s">
         <v>839</v>
@@ -39808,7 +39780,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1921">
-      <c r="A1921" s="18"/>
       <c r="B1921" s="21" t="s">
         <v>815</v>
       </c>
@@ -39823,7 +39794,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1922">
-      <c r="A1922" s="18"/>
       <c r="B1922" s="21" t="s">
         <v>799</v>
       </c>
@@ -39838,7 +39808,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1923">
-      <c r="A1923" s="18"/>
       <c r="B1923" s="21" t="s">
         <v>797</v>
       </c>
@@ -40415,7 +40384,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1964">
       <c r="A1964" s="18" t="s">
-        <v>595</v>
+        <v>673</v>
       </c>
       <c r="B1964" s="21" t="s">
         <v>839</v>
@@ -40515,7 +40484,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1971">
-      <c r="A1971" s="18"/>
       <c r="B1971" s="21" t="s">
         <v>799</v>
       </c>
@@ -40530,7 +40498,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1972">
-      <c r="A1972" s="18"/>
       <c r="B1972" s="21" t="s">
         <v>797</v>
       </c>
@@ -40545,7 +40512,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1973">
-      <c r="A1973" s="18"/>
       <c r="B1973" s="21" t="s">
         <v>800</v>
       </c>
@@ -41102,2076 +41068,6 @@
         <v>11</v>
       </c>
       <c r="E2012" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2013">
-      <c r="A2013" s="18" t="s">
-        <v>642</v>
-      </c>
-      <c r="B2013" s="21" t="s">
-        <v>839</v>
-      </c>
-      <c r="C2013" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2013" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2013" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2014">
-      <c r="B2014" s="21" t="s">
-        <v>787</v>
-      </c>
-      <c r="C2014" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2014" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2014" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2015">
-      <c r="B2015" s="21" t="s">
-        <v>876</v>
-      </c>
-      <c r="C2015" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2015" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2015" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2016">
-      <c r="B2016" s="21" t="s">
-        <v>790</v>
-      </c>
-      <c r="C2016" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2016" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2016" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2017">
-      <c r="B2017" s="21" t="s">
-        <v>795</v>
-      </c>
-      <c r="C2017" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2017" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2017" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2018">
-      <c r="B2018" s="21" t="s">
-        <v>865</v>
-      </c>
-      <c r="C2018" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2018" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2018" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2019">
-      <c r="B2019" s="21" t="s">
-        <v>815</v>
-      </c>
-      <c r="C2019" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2019" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2019" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2020">
-      <c r="B2020" s="21" t="s">
-        <v>799</v>
-      </c>
-      <c r="C2020" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2020" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2020" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2021">
-      <c r="A2021" s="18"/>
-      <c r="B2021" s="21" t="s">
-        <v>797</v>
-      </c>
-      <c r="C2021" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2021" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2021" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2022">
-      <c r="A2022" s="18"/>
-      <c r="B2022" s="21" t="s">
-        <v>800</v>
-      </c>
-      <c r="C2022" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2022" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2022" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2023">
-      <c r="B2023" s="21" t="s">
-        <v>802</v>
-      </c>
-      <c r="C2023" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2023" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2023" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2024">
-      <c r="B2024" s="21" t="s">
-        <v>849</v>
-      </c>
-      <c r="C2024" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2024" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2024" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2025">
-      <c r="B2025" s="21" t="s">
-        <v>863</v>
-      </c>
-      <c r="C2025" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2025" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2025" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2026">
-      <c r="B2026" s="21" t="s">
-        <v>805</v>
-      </c>
-      <c r="C2026" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2026" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2026" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2027">
-      <c r="B2027" s="21" t="s">
-        <v>890</v>
-      </c>
-      <c r="C2027" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2027" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2027" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2028">
-      <c r="B2028" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2028" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2028" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2028" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2029">
-      <c r="B2029" s="21" t="s">
-        <v>910</v>
-      </c>
-      <c r="C2029" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2029" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2029" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2030">
-      <c r="B2030" s="21" t="s">
-        <v>807</v>
-      </c>
-      <c r="C2030" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2030" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2030" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2031">
-      <c r="B2031" s="21" t="s">
-        <v>912</v>
-      </c>
-      <c r="C2031" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2031" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2031" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2032">
-      <c r="B2032" s="21" t="s">
-        <v>820</v>
-      </c>
-      <c r="C2032" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2032" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2032" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2033">
-      <c r="B2033" s="21" t="s">
-        <v>809</v>
-      </c>
-      <c r="C2033" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2033" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2033" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2034">
-      <c r="B2034" s="21" t="s">
-        <v>822</v>
-      </c>
-      <c r="C2034" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2034" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2034" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2035">
-      <c r="B2035" s="21" t="s">
-        <v>812</v>
-      </c>
-      <c r="C2035" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2035" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2035" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2036">
-      <c r="B2036" s="21" t="s">
-        <v>844</v>
-      </c>
-      <c r="C2036" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2036" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2036" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2037">
-      <c r="B2037" s="21" t="s">
-        <v>823</v>
-      </c>
-      <c r="C2037" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2037" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2037" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2038">
-      <c r="B2038" s="21" t="s">
-        <v>881</v>
-      </c>
-      <c r="C2038" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2038" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2038" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2039">
-      <c r="B2039" s="21" t="s">
-        <v>825</v>
-      </c>
-      <c r="C2039" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2039" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2039" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2040">
-      <c r="B2040" s="21" t="s">
-        <v>827</v>
-      </c>
-      <c r="C2040" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2040" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2040" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2041">
-      <c r="B2041" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2041" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2041" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2041" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2042">
-      <c r="B2042" s="21" t="s">
-        <v>831</v>
-      </c>
-      <c r="C2042" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2042" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2042" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2043">
-      <c r="B2043" s="21" t="s">
-        <v>851</v>
-      </c>
-      <c r="C2043" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2043" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2043" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2044">
-      <c r="B2044" s="21" t="s">
-        <v>817</v>
-      </c>
-      <c r="C2044" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2044" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2044" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2045">
-      <c r="B2045" s="21" t="s">
-        <v>841</v>
-      </c>
-      <c r="C2045" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2045" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2045" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2046">
-      <c r="B2046" s="21" t="s">
-        <v>886</v>
-      </c>
-      <c r="C2046" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2046" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2046" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2047">
-      <c r="B2047" s="21" t="s">
-        <v>835</v>
-      </c>
-      <c r="C2047" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2047" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2047" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2048">
-      <c r="B2048" s="21" t="s">
-        <v>784</v>
-      </c>
-      <c r="C2048" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2048" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2048" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2049">
-      <c r="B2049" s="21" t="s">
-        <v>833</v>
-      </c>
-      <c r="C2049" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2049" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2049" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2050">
-      <c r="B2050" s="21" t="s">
-        <v>837</v>
-      </c>
-      <c r="C2050" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2050" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2050" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2051">
-      <c r="B2051" s="21" t="s">
-        <v>858</v>
-      </c>
-      <c r="C2051" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2051" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2051" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2052">
-      <c r="B2052" s="21" t="s">
-        <v>847</v>
-      </c>
-      <c r="C2052" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2052" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2052" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2053">
-      <c r="B2053" s="21" t="s">
-        <v>861</v>
-      </c>
-      <c r="C2053" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2053" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2053" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2054">
-      <c r="B2054" s="21" t="s">
-        <v>853</v>
-      </c>
-      <c r="C2054" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2054" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2054" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2055">
-      <c r="B2055" s="21" t="s">
-        <v>856</v>
-      </c>
-      <c r="C2055" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2055" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2055" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2056">
-      <c r="B2056" s="21" t="s">
-        <v>894</v>
-      </c>
-      <c r="C2056" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2056" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2056" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2057">
-      <c r="B2057" s="21" t="s">
-        <v>775</v>
-      </c>
-      <c r="C2057" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2057" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2057" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2058">
-      <c r="B2058" s="21" t="s">
-        <v>867</v>
-      </c>
-      <c r="C2058" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2058" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2058" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2059">
-      <c r="B2059" s="21" t="s">
-        <v>914</v>
-      </c>
-      <c r="C2059" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2059" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2059" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2060">
-      <c r="B2060" s="21" t="s">
-        <v>868</v>
-      </c>
-      <c r="C2060" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2060" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2060" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2061">
-      <c r="B2061" s="21" t="s">
-        <v>870</v>
-      </c>
-      <c r="C2061" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2061" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2061" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2062">
-      <c r="A2062" s="18" t="s">
-        <v>669</v>
-      </c>
-      <c r="B2062" s="21" t="s">
-        <v>839</v>
-      </c>
-      <c r="C2062" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2062" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2062" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2063">
-      <c r="B2063" s="21" t="s">
-        <v>787</v>
-      </c>
-      <c r="C2063" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2063" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2063" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2064">
-      <c r="B2064" s="21" t="s">
-        <v>876</v>
-      </c>
-      <c r="C2064" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2064" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2064" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2065">
-      <c r="B2065" s="21" t="s">
-        <v>790</v>
-      </c>
-      <c r="C2065" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2065" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2065" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2066">
-      <c r="B2066" s="21" t="s">
-        <v>795</v>
-      </c>
-      <c r="C2066" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2066" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2066" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2067">
-      <c r="B2067" s="21" t="s">
-        <v>865</v>
-      </c>
-      <c r="C2067" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2067" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2067" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2068">
-      <c r="B2068" s="21" t="s">
-        <v>815</v>
-      </c>
-      <c r="C2068" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2068" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2068" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2069">
-      <c r="B2069" s="21" t="s">
-        <v>799</v>
-      </c>
-      <c r="C2069" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2069" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2069" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2070">
-      <c r="B2070" s="21" t="s">
-        <v>797</v>
-      </c>
-      <c r="C2070" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2070" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2070" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2071">
-      <c r="A2071" s="18"/>
-      <c r="B2071" s="21" t="s">
-        <v>800</v>
-      </c>
-      <c r="C2071" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2071" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2071" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2072">
-      <c r="B2072" s="21" t="s">
-        <v>802</v>
-      </c>
-      <c r="C2072" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2072" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2072" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2073">
-      <c r="B2073" s="21" t="s">
-        <v>849</v>
-      </c>
-      <c r="C2073" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2073" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2073" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2074">
-      <c r="B2074" s="21" t="s">
-        <v>863</v>
-      </c>
-      <c r="C2074" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2074" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2074" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2075">
-      <c r="B2075" s="21" t="s">
-        <v>805</v>
-      </c>
-      <c r="C2075" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2075" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2075" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2076">
-      <c r="B2076" s="21" t="s">
-        <v>890</v>
-      </c>
-      <c r="C2076" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2076" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2076" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2077">
-      <c r="B2077" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2077" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2077" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2077" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2078">
-      <c r="B2078" s="21" t="s">
-        <v>910</v>
-      </c>
-      <c r="C2078" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2078" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2078" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2079">
-      <c r="B2079" s="21" t="s">
-        <v>807</v>
-      </c>
-      <c r="C2079" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2079" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2079" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2080">
-      <c r="B2080" s="21" t="s">
-        <v>912</v>
-      </c>
-      <c r="C2080" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2080" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2080" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2081">
-      <c r="B2081" s="21" t="s">
-        <v>820</v>
-      </c>
-      <c r="C2081" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2081" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2081" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2082">
-      <c r="B2082" s="21" t="s">
-        <v>809</v>
-      </c>
-      <c r="C2082" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2082" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2082" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2083">
-      <c r="B2083" s="21" t="s">
-        <v>822</v>
-      </c>
-      <c r="C2083" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2083" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2083" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2084">
-      <c r="B2084" s="21" t="s">
-        <v>812</v>
-      </c>
-      <c r="C2084" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2084" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2084" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2085">
-      <c r="B2085" s="21" t="s">
-        <v>844</v>
-      </c>
-      <c r="C2085" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2085" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2085" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2086">
-      <c r="B2086" s="21" t="s">
-        <v>823</v>
-      </c>
-      <c r="C2086" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2086" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2086" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2087">
-      <c r="B2087" s="21" t="s">
-        <v>881</v>
-      </c>
-      <c r="C2087" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2087" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2087" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2088">
-      <c r="B2088" s="21" t="s">
-        <v>825</v>
-      </c>
-      <c r="C2088" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2088" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2088" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2089">
-      <c r="B2089" s="21" t="s">
-        <v>827</v>
-      </c>
-      <c r="C2089" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2089" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2089" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2090">
-      <c r="B2090" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2090" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2090" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2090" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2091">
-      <c r="B2091" s="21" t="s">
-        <v>831</v>
-      </c>
-      <c r="C2091" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2091" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2091" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2092">
-      <c r="B2092" s="21" t="s">
-        <v>851</v>
-      </c>
-      <c r="C2092" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2092" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2092" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2093">
-      <c r="B2093" s="21" t="s">
-        <v>817</v>
-      </c>
-      <c r="C2093" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2093" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2093" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2094">
-      <c r="B2094" s="21" t="s">
-        <v>841</v>
-      </c>
-      <c r="C2094" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2094" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2094" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2095">
-      <c r="B2095" s="21" t="s">
-        <v>886</v>
-      </c>
-      <c r="C2095" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2095" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2095" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2096">
-      <c r="B2096" s="21" t="s">
-        <v>835</v>
-      </c>
-      <c r="C2096" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2096" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2096" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2097">
-      <c r="B2097" s="21" t="s">
-        <v>784</v>
-      </c>
-      <c r="C2097" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2097" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2097" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2098">
-      <c r="B2098" s="21" t="s">
-        <v>833</v>
-      </c>
-      <c r="C2098" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2098" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2098" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2099">
-      <c r="B2099" s="21" t="s">
-        <v>837</v>
-      </c>
-      <c r="C2099" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2099" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2099" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2100">
-      <c r="B2100" s="21" t="s">
-        <v>858</v>
-      </c>
-      <c r="C2100" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2100" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2100" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2101">
-      <c r="B2101" s="21" t="s">
-        <v>847</v>
-      </c>
-      <c r="C2101" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2101" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2101" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2102">
-      <c r="B2102" s="21" t="s">
-        <v>861</v>
-      </c>
-      <c r="C2102" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2102" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2102" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2103">
-      <c r="B2103" s="21" t="s">
-        <v>853</v>
-      </c>
-      <c r="C2103" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2103" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2103" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2104">
-      <c r="B2104" s="21" t="s">
-        <v>856</v>
-      </c>
-      <c r="C2104" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2104" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2104" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2105">
-      <c r="B2105" s="21" t="s">
-        <v>894</v>
-      </c>
-      <c r="C2105" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2105" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2105" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2106">
-      <c r="B2106" s="21" t="s">
-        <v>775</v>
-      </c>
-      <c r="C2106" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2106" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2106" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2107">
-      <c r="B2107" s="21" t="s">
-        <v>867</v>
-      </c>
-      <c r="C2107" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2107" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2107" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2108">
-      <c r="B2108" s="21" t="s">
-        <v>914</v>
-      </c>
-      <c r="C2108" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2108" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2108" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2109">
-      <c r="B2109" s="21" t="s">
-        <v>868</v>
-      </c>
-      <c r="C2109" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2109" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2109" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2110">
-      <c r="B2110" s="21" t="s">
-        <v>870</v>
-      </c>
-      <c r="C2110" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2110" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2110" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2111">
-      <c r="A2111" s="18" t="s">
-        <v>673</v>
-      </c>
-      <c r="B2111" s="21" t="s">
-        <v>839</v>
-      </c>
-      <c r="C2111" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2111" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2111" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2112">
-      <c r="B2112" s="21" t="s">
-        <v>787</v>
-      </c>
-      <c r="C2112" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2112" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2112" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2113">
-      <c r="B2113" s="21" t="s">
-        <v>876</v>
-      </c>
-      <c r="C2113" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2113" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2113" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2114">
-      <c r="B2114" s="21" t="s">
-        <v>790</v>
-      </c>
-      <c r="C2114" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2114" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2114" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2115">
-      <c r="B2115" s="21" t="s">
-        <v>795</v>
-      </c>
-      <c r="C2115" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2115" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2115" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2116">
-      <c r="B2116" s="21" t="s">
-        <v>865</v>
-      </c>
-      <c r="C2116" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2116" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2116" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2117">
-      <c r="B2117" s="21" t="s">
-        <v>815</v>
-      </c>
-      <c r="C2117" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2117" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2117" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2118">
-      <c r="B2118" s="21" t="s">
-        <v>799</v>
-      </c>
-      <c r="C2118" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2118" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2118" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2119">
-      <c r="B2119" s="21" t="s">
-        <v>797</v>
-      </c>
-      <c r="C2119" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2119" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2119" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2120">
-      <c r="B2120" s="21" t="s">
-        <v>800</v>
-      </c>
-      <c r="C2120" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2120" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2120" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2121">
-      <c r="B2121" s="21" t="s">
-        <v>802</v>
-      </c>
-      <c r="C2121" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2121" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2121" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2122">
-      <c r="B2122" s="21" t="s">
-        <v>849</v>
-      </c>
-      <c r="C2122" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2122" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2122" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2123">
-      <c r="B2123" s="21" t="s">
-        <v>863</v>
-      </c>
-      <c r="C2123" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2123" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2123" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2124">
-      <c r="B2124" s="21" t="s">
-        <v>805</v>
-      </c>
-      <c r="C2124" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2124" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2124" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2125">
-      <c r="B2125" s="21" t="s">
-        <v>890</v>
-      </c>
-      <c r="C2125" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2125" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2125" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2126">
-      <c r="B2126" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2126" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2126" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2126" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2127">
-      <c r="B2127" s="21" t="s">
-        <v>910</v>
-      </c>
-      <c r="C2127" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2127" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2127" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2128">
-      <c r="B2128" s="21" t="s">
-        <v>807</v>
-      </c>
-      <c r="C2128" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2128" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2128" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2129">
-      <c r="B2129" s="21" t="s">
-        <v>912</v>
-      </c>
-      <c r="C2129" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2129" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2129" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2130">
-      <c r="B2130" s="21" t="s">
-        <v>820</v>
-      </c>
-      <c r="C2130" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2130" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2130" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2131">
-      <c r="B2131" s="21" t="s">
-        <v>809</v>
-      </c>
-      <c r="C2131" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2131" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2131" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2132">
-      <c r="B2132" s="21" t="s">
-        <v>822</v>
-      </c>
-      <c r="C2132" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2132" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2132" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2133">
-      <c r="B2133" s="21" t="s">
-        <v>812</v>
-      </c>
-      <c r="C2133" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2133" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2133" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2134">
-      <c r="B2134" s="21" t="s">
-        <v>844</v>
-      </c>
-      <c r="C2134" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2134" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2134" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2135">
-      <c r="B2135" s="21" t="s">
-        <v>823</v>
-      </c>
-      <c r="C2135" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2135" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2135" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2136">
-      <c r="B2136" s="21" t="s">
-        <v>881</v>
-      </c>
-      <c r="C2136" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2136" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2136" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2137">
-      <c r="B2137" s="21" t="s">
-        <v>825</v>
-      </c>
-      <c r="C2137" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2137" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2137" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2138">
-      <c r="B2138" s="21" t="s">
-        <v>827</v>
-      </c>
-      <c r="C2138" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2138" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2138" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2139">
-      <c r="B2139" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2139" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2139" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2139" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2140">
-      <c r="B2140" s="21" t="s">
-        <v>831</v>
-      </c>
-      <c r="C2140" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2140" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2140" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2141">
-      <c r="B2141" s="21" t="s">
-        <v>851</v>
-      </c>
-      <c r="C2141" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2141" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2141" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2142">
-      <c r="B2142" s="21" t="s">
-        <v>817</v>
-      </c>
-      <c r="C2142" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2142" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2142" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2143">
-      <c r="B2143" s="21" t="s">
-        <v>841</v>
-      </c>
-      <c r="C2143" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2143" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2143" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2144">
-      <c r="B2144" s="21" t="s">
-        <v>886</v>
-      </c>
-      <c r="C2144" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2144" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2144" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2145">
-      <c r="B2145" s="21" t="s">
-        <v>835</v>
-      </c>
-      <c r="C2145" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2145" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2145" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2146">
-      <c r="B2146" s="21" t="s">
-        <v>784</v>
-      </c>
-      <c r="C2146" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2146" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2146" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2147">
-      <c r="B2147" s="21" t="s">
-        <v>833</v>
-      </c>
-      <c r="C2147" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2147" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2147" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2148">
-      <c r="B2148" s="21" t="s">
-        <v>837</v>
-      </c>
-      <c r="C2148" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2148" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2148" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2149">
-      <c r="B2149" s="21" t="s">
-        <v>858</v>
-      </c>
-      <c r="C2149" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2149" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2149" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2150">
-      <c r="B2150" s="21" t="s">
-        <v>847</v>
-      </c>
-      <c r="C2150" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2150" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2150" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2151">
-      <c r="B2151" s="21" t="s">
-        <v>861</v>
-      </c>
-      <c r="C2151" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2151" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2151" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2152">
-      <c r="B2152" s="21" t="s">
-        <v>853</v>
-      </c>
-      <c r="C2152" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2152" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2152" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2153">
-      <c r="B2153" s="21" t="s">
-        <v>856</v>
-      </c>
-      <c r="C2153" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2153" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2153" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2154">
-      <c r="B2154" s="21" t="s">
-        <v>894</v>
-      </c>
-      <c r="C2154" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2154" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2154" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2155">
-      <c r="B2155" s="21" t="s">
-        <v>775</v>
-      </c>
-      <c r="C2155" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2155" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2155" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2156">
-      <c r="B2156" s="21" t="s">
-        <v>867</v>
-      </c>
-      <c r="C2156" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2156" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2156" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2157">
-      <c r="B2157" s="21" t="s">
-        <v>914</v>
-      </c>
-      <c r="C2157" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2157" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2157" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2158">
-      <c r="B2158" s="21" t="s">
-        <v>868</v>
-      </c>
-      <c r="C2158" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2158" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2158" s="28" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2159">
-      <c r="B2159" s="21" t="s">
-        <v>870</v>
-      </c>
-      <c r="C2159" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2159" s="28" t="n">
-        <v>11</v>
-      </c>
-      <c r="E2159" s="28" t="n">
         <v>10</v>
       </c>
     </row>
@@ -43194,15 +41090,15 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B15" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D29" activeCellId="0" pane="topLeft" sqref="A17:G66"/>
+      <selection activeCell="D29" activeCellId="0" pane="topLeft" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="61.6352941176471"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="29.8117647058824"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="32.9921568627451"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="8" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="61.9450980392157"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="29.9647058823529"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="33.156862745098"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="8" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="1" s="9">
@@ -43535,7 +41431,7 @@
         <v>947</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="15">
       <c r="A15" s="28" t="s">
         <v>818</v>
       </c>
@@ -43898,12 +41794,12 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="29.6470588235294"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="0" width="10.7254901960784"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="29.7921568627451"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="0" width="10.7803921568627"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="40">
@@ -44035,13 +41931,13 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B1" activeCellId="1" pane="topLeft" sqref="A17:G66 B1"/>
+      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="31.156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="60.2980392156863"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="31.3098039215686"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="60.5960784313726"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="11">
@@ -44121,12 +42017,12 @@
   <dimension ref="A1:W79"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="27.6392156862745"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="28" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="27.7764705882353"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="28" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="27">
@@ -45362,15 +43258,15 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="31" width="18.2509803921569"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="31" width="27.6392156862745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="31" width="30.6509803921569"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="31" width="26.2901960784314"/>
-    <col collapsed="false" hidden="false" max="257" min="6" style="31" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="31" width="18.3411764705882"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="31" width="27.7764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="31" width="30.8039215686275"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="31" width="26.4196078431373"/>
+    <col collapsed="false" hidden="false" max="257" min="6" style="31" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="32">
@@ -45519,17 +43415,17 @@
   <dimension ref="A2:M4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="14.9058823529412"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="5" width="11.3882352941176"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="25.4588235294118"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="25.1254901960784"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="5" width="14.9058823529412"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="5" width="23.1176470588235"/>
-    <col collapsed="false" hidden="false" max="257" min="14" style="5" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="14.9882352941176"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="5" width="11.4392156862745"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="25.5882352941176"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="25.2509803921569"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="5" width="14.9882352941176"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="5" width="23.2352941176471"/>
+    <col collapsed="false" hidden="false" max="257" min="14" style="5" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2" s="2"/>
@@ -45640,14 +43536,14 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="31" width="24.121568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="31" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="31" width="22.7725490196078"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="31" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="31" width="24.2392156862745"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="31" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="31" width="22.8823529411765"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="31" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="32">
@@ -45793,12 +43689,12 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="8" width="32.1607843137255"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="8" width="32.3254901960784"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="11">
@@ -45894,13 +43790,13 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="44.8862745098039"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="36.0156862745098"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="45.1137254901961"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="36.1960784313725"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="11">
@@ -46297,15 +44193,15 @@
   <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A27" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="28" width="18.9294117647059"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="28" width="22.1137254901961"/>
-    <col collapsed="false" hidden="false" max="8" min="4" style="28" width="18.9294117647059"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="10.7254901960784"/>
-    <col collapsed="false" hidden="false" max="257" min="12" style="28" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="28" width="19.0196078431373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="28" width="22.2235294117647"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="28" width="19.0196078431373"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="10.7803921568627"/>
+    <col collapsed="false" hidden="false" max="257" min="12" style="28" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="27">
@@ -46794,12 +44690,12 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="32.4980392156863"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="8" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="32.6588235294118"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="8" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="11">
@@ -46956,15 +44852,15 @@
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A17" activeCellId="0" pane="topLeft" sqref="A17:G66"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E22" activeCellId="0" pane="topLeft" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="8" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="25.1254901960784"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="24.6196078431373"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="8" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="25.2509803921569"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="24.7372549019608"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="8" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="10">
@@ -47336,17 +45232,17 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K1" activeCellId="1" pane="topLeft" sqref="A17:G66 K1"/>
+      <selection activeCell="K1" activeCellId="0" pane="topLeft" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="8" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="22.1137254901961"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="8" width="18.756862745098"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="21.7686274509804"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="24.4549019607843"/>
-    <col collapsed="false" hidden="false" max="257" min="12" style="8" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="22.2235294117647"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="8" width="18.8470588235294"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="21.878431372549"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="24.5725490196078"/>
+    <col collapsed="false" hidden="false" max="257" min="12" style="8" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="11">
@@ -47688,13 +45584,13 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A17:G66 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="29.3137254901961"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="8" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="29.4588235294118"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="8" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="9">
@@ -47779,15 +45675,15 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="27.9725490196078"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="26.4627450980392"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="13" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="28.1098039215686"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="26.6"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="13" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="11.6" outlineLevel="0" r="1" s="16">
@@ -48048,19 +45944,19 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="17.2470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="13" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="19.9333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="20.9372549019608"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="13" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="13" width="23.4509803921569"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="13" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="17" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="257" min="17" style="13" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="17.3294117647059"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="13" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="20.0313725490196"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="21.0470588235294"/>
+    <col collapsed="false" hidden="false" max="12" min="7" style="13" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="13" width="23.5686274509804"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="13" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="17" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="257" min="17" style="13" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="11.6" outlineLevel="0" r="1" s="16">
@@ -49122,17 +47018,17 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="21.4352941176471"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="36.8470588235294"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="22.1137254901961"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="18" width="19.7607843137255"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="18" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="18" width="18.9294117647059"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="18" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="21.5450980392157"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="37.0274509803922"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="22.2235294117647"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="18" width="19.8627450980392"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="18" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="18" width="19.0196078431373"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="18" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="20">
@@ -49766,13 +47662,13 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A17:G66 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="23.1176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="24.2823529411765"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="23.2352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="24.4"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="10.9450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="13" outlineLevel="0" r="1" s="9">

</xml_diff>

<commit_message>
Remove prefixes from setup data
added sane defaults to bikasetup.py
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test.xlsx
+++ b/bika/lims/setupdata/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="13" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="969" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="22" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="958" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,14 +31,13 @@
     <sheet name="Attachment Types" sheetId="21" state="visible" r:id="rId22"/>
     <sheet name="Lab Products" sheetId="22" state="visible" r:id="rId23"/>
     <sheet name="Worksheet Templates" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="Prefixes" sheetId="24" state="visible" r:id="rId25"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4526" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4503" uniqueCount="1111">
   <si>
     <t>Password lifetime</t>
   </si>
@@ -1675,7 +1674,7 @@
     <t>Public lake</t>
   </si>
   <si>
-    <t>Shop – BB Supermarket</t>
+    <t>Shop - BB Supermarket</t>
   </si>
   <si>
     <t>From the shelves</t>
@@ -2662,7 +2661,7 @@
     <t>7.5</t>
   </si>
   <si>
-    <t>AME – Apparent Metabolisable Energy</t>
+    <t>AME - Apparent Metabolisable Energy</t>
   </si>
   <si>
     <t>AME used for poultry feed as no correction is made for faecal or endogenous energy losses</t>
@@ -2677,7 +2676,7 @@
     <t>Apparent Metabolisable Energy</t>
   </si>
   <si>
-    <t>ME – Metabolisable Energy</t>
+    <t>ME - Metabolisable Energy</t>
   </si>
   <si>
     <t>ME used for ruminant feeds</t>
@@ -2704,7 +2703,7 @@
     <t>% DM</t>
   </si>
   <si>
-    <t>DE – Digestible Energy</t>
+    <t>DE - Digestible Energy</t>
   </si>
   <si>
     <t>DE is used for pig feeds</t>
@@ -3371,66 +3370,6 @@
   </si>
   <si>
     <t>ME,CP,EE,CF,Ash</t>
-  </si>
-  <si>
-    <t>Prefixes</t>
-  </si>
-  <si>
-    <t>portal_type</t>
-  </si>
-  <si>
-    <t>prefix</t>
-  </si>
-  <si>
-    <t>padding</t>
-  </si>
-  <si>
-    <t>Portal Type</t>
-  </si>
-  <si>
-    <t>Padding</t>
-  </si>
-  <si>
-    <t>ARImport</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>client</t>
-  </si>
-  <si>
-    <t>DuplicateAnalysis</t>
-  </si>
-  <si>
-    <t>DA</t>
-  </si>
-  <si>
-    <t>Invoice</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>ReferenceAnalysis</t>
-  </si>
-  <si>
-    <t>RA</t>
-  </si>
-  <si>
-    <t>ReferenceSample</t>
-  </si>
-  <si>
-    <t>RS</t>
-  </si>
-  <si>
-    <t>SupplyOrder</t>
-  </si>
-  <si>
-    <t>Worksheet</t>
-  </si>
-  <si>
-    <t>WS</t>
   </si>
 </sst>
 </file>
@@ -3815,7 +3754,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2" s="2"/>
@@ -3927,11 +3866,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="20.1960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="39.5607843137255"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="18.8470588235294"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="20.3960784313725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="39.956862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="19.0274509803922"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="8" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="9">
@@ -4756,9 +4695,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="31" width="33.3294117647059"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="31" width="51.6705882352941"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="31" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="31" width="33.6627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="31" width="52.1843137254902"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="31" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="32">
@@ -4909,10 +4848,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="82.1411764705882"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="23.7333333333333"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="82.9647058823529"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="23.9686274509804"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="8" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="9">
@@ -5135,22 +5074,22 @@
   </sheetPr>
   <dimension ref="A1:AB271"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="G1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" topLeftCell="A248" xSplit="0" ySplit="1185"/>
-      <selection activeCell="G1" activeCellId="0" pane="topLeft" sqref="G1"/>
-      <selection activeCell="Q263" activeCellId="0" pane="bottomLeft" sqref="Q263"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="bottomLeft" topLeftCell="A198" xSplit="0" ySplit="1185"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="I210" activeCellId="0" pane="bottomLeft" sqref="I210"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="21" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="34" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="20" min="8" style="21" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="34" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="21" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="18" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="21" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="28" min="25" style="8" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="257" min="29" style="28" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="21" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="34" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="20" min="8" style="21" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="34" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="21" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="18" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="21" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="28" min="25" style="8" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="257" min="29" style="28" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24.25" outlineLevel="0" r="1" s="23">
@@ -11855,14 +11794,14 @@
   </sheetPr>
   <dimension ref="A1:E2012"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1963" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E2009" activeCellId="0" pane="topLeft" sqref="E2009"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1963" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D1991" activeCellId="0" pane="topLeft" sqref="D1991"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="21" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="227" min="4" style="28" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="257" min="228" style="0" width="10.7803921568627"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="21" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="227" min="4" style="28" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="257" min="228" style="0" width="10.8901960784314"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24.25" outlineLevel="0" r="1" s="23">
@@ -41094,11 +41033,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="61.9450980392157"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="29.9647058823529"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="33.156862745098"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="62.5607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="30.2705882352941"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="33.4823529411765"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="8" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="1" s="9">
@@ -41798,8 +41737,8 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="29.7921568627451"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="0" width="10.7803921568627"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="30.0901960784314"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="0" width="10.8901960784314"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="40">
@@ -41935,9 +41874,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="31.3098039215686"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="60.5960784313726"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="31.6196078431373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="61.1921568627451"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="11">
@@ -42021,8 +41960,8 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="27.7764705882353"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="28" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="28.0470588235294"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="28" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="27">
@@ -43262,11 +43201,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="31" width="18.3411764705882"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="31" width="27.7764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="31" width="30.8039215686275"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="31" width="26.4196078431373"/>
-    <col collapsed="false" hidden="false" max="257" min="6" style="31" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="31" width="18.521568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="31" width="28.0470588235294"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="31" width="31.1137254901961"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="31" width="26.6823529411765"/>
+    <col collapsed="false" hidden="false" max="257" min="6" style="31" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="32">
@@ -43419,13 +43358,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="14.9882352941176"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="5" width="11.4392156862745"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="25.5882352941176"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="25.2509803921569"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="5" width="14.9882352941176"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="5" width="23.2352941176471"/>
-    <col collapsed="false" hidden="false" max="257" min="14" style="5" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="15.1411764705882"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="5" width="11.5490196078431"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="25.8392156862745"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="25.5058823529412"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="5" width="15.1411764705882"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="5" width="23.4705882352941"/>
+    <col collapsed="false" hidden="false" max="257" min="14" style="5" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2" s="2"/>
@@ -43470,7 +43409,7 @@
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
@@ -43540,10 +43479,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="31" width="24.2392156862745"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="31" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="31" width="22.8823529411765"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="31" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="31" width="24.4823529411765"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="31" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="31" width="23.1176470588235"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="31" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="32">
@@ -43693,8 +43632,8 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="8" width="32.3254901960784"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="8" width="32.6509803921569"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="11">
@@ -43794,9 +43733,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="45.1137254901961"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="36.1960784313725"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="45.5647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="36.556862745098"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="11">
@@ -44192,16 +44131,16 @@
   </sheetPr>
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A27" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A27" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E45" activeCellId="0" pane="topLeft" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="28" width="19.0196078431373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="28" width="22.2235294117647"/>
-    <col collapsed="false" hidden="false" max="8" min="4" style="28" width="19.0196078431373"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="10.7803921568627"/>
-    <col collapsed="false" hidden="false" max="257" min="12" style="28" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="28" width="19.2196078431373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="28" width="22.4588235294118"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="28" width="19.2196078431373"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="10.8901960784314"/>
+    <col collapsed="false" hidden="false" max="257" min="12" style="28" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="27">
@@ -44668,169 +44607,6 @@
         <v>1108</v>
       </c>
       <c r="H43" s="28" t="n">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:V11"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="32.6588235294118"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="8" width="10.9450980392157"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="11">
-      <c r="A1" s="23" t="s">
-        <v>1111</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2" s="2">
-      <c r="A2" s="2" t="s">
-        <v>1112</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1113</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1114</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3" s="3">
-      <c r="A3" s="3" t="s">
-        <v>1115</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1116</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
-      <c r="A4" s="28" t="s">
-        <v>1117</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>1118</v>
-      </c>
-      <c r="C4" s="28" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
-      <c r="A5" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>1119</v>
-      </c>
-      <c r="C5" s="28" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
-      <c r="A6" s="28" t="s">
-        <v>1120</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C6" s="28" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
-      <c r="A7" s="28" t="s">
-        <v>1122</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>1123</v>
-      </c>
-      <c r="C7" s="28" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
-      <c r="A8" s="28" t="s">
-        <v>1124</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>1125</v>
-      </c>
-      <c r="C8" s="28" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
-      <c r="A9" s="28" t="s">
-        <v>1126</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C9" s="28" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
-      <c r="A10" s="28" t="s">
-        <v>1128</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>643</v>
-      </c>
-      <c r="C10" s="28" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
-      <c r="A11" s="28" t="s">
-        <v>1129</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>1130</v>
-      </c>
-      <c r="C11" s="28" t="n">
         <v>3</v>
       </c>
     </row>
@@ -44857,10 +44633,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="8" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="25.2509803921569"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="24.7372549019608"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="8" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="25.5058823529412"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="24.9882352941176"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="8" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="10">
@@ -45236,13 +45012,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="8" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="22.2235294117647"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="8" width="18.8470588235294"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="21.878431372549"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="24.5725490196078"/>
-    <col collapsed="false" hidden="false" max="257" min="12" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="8" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="22.4588235294118"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="8" width="19.0274509803922"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="22.0941176470588"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="24.8078431372549"/>
+    <col collapsed="false" hidden="false" max="257" min="12" style="8" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="11">
@@ -45588,9 +45364,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="29.4588235294118"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="29.7450980392157"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="8" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="9">
@@ -45679,11 +45455,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="28.1098039215686"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="26.6"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="13" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="28.4"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="26.8705882352941"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="13" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="11.6" outlineLevel="0" r="1" s="16">
@@ -45948,15 +45724,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="17.3294117647059"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="13" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="20.0313725490196"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="21.0470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="13" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="13" width="23.5686274509804"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="13" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="17" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="257" min="17" style="13" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="17.5019607843137"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="13" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="20.2313725490196"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="21.2549019607843"/>
+    <col collapsed="false" hidden="false" max="12" min="7" style="13" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="13" width="23.8039215686274"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="13" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="17" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="257" min="17" style="13" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="11.6" outlineLevel="0" r="1" s="16">
@@ -47022,13 +46798,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="21.5450980392157"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="37.0274509803922"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="22.2235294117647"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="18" width="19.8627450980392"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="18" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="18" width="19.0196078431373"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="18" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="21.7607843137255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="37.4"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="22.4588235294118"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="18" width="20.0588235294118"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="18" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="18" width="19.2196078431373"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="18" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="20">
@@ -47666,9 +47442,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="23.2352941176471"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="24.4"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="23.4705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="24.6352941176471"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="8" width="11.0509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="13" outlineLevel="0" r="1" s="9">

</xml_diff>